<commit_message>
Update the excel file to create the inventory inserts into the database
</commit_message>
<xml_diff>
--- a/Excelitems/items.xlsx
+++ b/Excelitems/items.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\WebProgrammingProject3\Excelitems\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="8475"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19152" windowHeight="8472"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t xml:space="preserve">itemname </t>
   </si>
@@ -33,9 +38,6 @@
     <t xml:space="preserve">numberinstock </t>
   </si>
   <si>
-    <t>backordered tinyint</t>
-  </si>
-  <si>
     <t>Batman Arkham Knight</t>
   </si>
   <si>
@@ -69,9 +71,6 @@
     <t>Watch Dogs</t>
   </si>
   <si>
-    <t>Call of Duty Ghosts - PlayStation 4.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Call of Duty Ghosts </t>
   </si>
   <si>
@@ -87,53 +86,63 @@
     <t>Flat Screen</t>
   </si>
   <si>
-    <t>WebProgrammingProject3 / images / Plants vs. Zombies Garden Warfare - Xbox One.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / The Last of Us Remastered - PlayStation 4.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Watch Dogs - PlayStation 4.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / NBA 2K14 - Xbox One.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Destiny - Xbox One.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Batman Arkham Knight.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Infamous Second Son - PlayStation 4.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / FIFA Soccer 14 (PS4).jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Samsung - 40 inch Class (40 inch Diag.) - LED-LCD TV - 1080p - HDTV 1080p.jpg</t>
-  </si>
-  <si>
-    <t> LG - 65 inch LED - 240Hz - Smart - 3D - HDTV</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / LG - 65 inch Class (64-5 a half 8inch Diag.) - LED - 4K Ultra HD TV (2160p) - 240Hz - Smart - 3D - HDTV.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Microsoft Xbox One.jpg</t>
-  </si>
-  <si>
-    <t>WebProgrammingProject3 / images / Sony - Playstation 4.jpg</t>
+    <t>images/Microsoft Xbox One.jpg</t>
+  </si>
+  <si>
+    <t>images/Batman Arkham Knight.jpg</t>
+  </si>
+  <si>
+    <t>images/Destiny - Xbox One.jpg</t>
+  </si>
+  <si>
+    <t>images/NBA 2K14 - Xbox One.jpg</t>
+  </si>
+  <si>
+    <t>images/Plants vs. Zombies Garden Warfare - Xbox One.jpg</t>
+  </si>
+  <si>
+    <t>images/Sony - Playstation 4.jpg</t>
+  </si>
+  <si>
+    <t>images/The Last of Us Remastered - PlayStation 4.jpg</t>
+  </si>
+  <si>
+    <t>images/Watch Dogs - PlayStation 4.jpg</t>
+  </si>
+  <si>
+    <t>images/Infamous Second Son - PlayStation 4.jpg</t>
+  </si>
+  <si>
+    <t>images/FIFA Soccer 14 (PS4).jpg</t>
+  </si>
+  <si>
+    <t>images/LG - 65 inch Class (64-5 a half 8inch Diag.) - LED - 4K Ultra HD TV (2160p) - 240Hz - Smart - 3D - HDTV.jpg</t>
+  </si>
+  <si>
+    <t>images/Samsung - 40 inch Class (40 inch Diag.) - LED-LCD TV - 1080p - HDTV 1080p.jpg</t>
+  </si>
+  <si>
+    <t>images/Call of Duty Ghosts - PlayStation 4.jpg</t>
+  </si>
+  <si>
+    <t>LG - 65 inch LED - 240Hz - Smart - 3D - HDTV</t>
+  </si>
+  <si>
+    <t>backordered</t>
+  </si>
+  <si>
+    <t>arrivaldate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,10 +185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -187,6 +198,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -233,7 +252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,9 +284,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,6 +319,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,25 +495,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="191.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="62.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,18 +531,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f>"insert into inventory("&amp;A1&amp;","&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;","&amp;E1&amp;","&amp;F1&amp;","&amp;G1&amp;") values "</f>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values </v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2">
         <v>599</v>
@@ -531,16 +560,27 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="4">
+        <v>41809.907581539119</v>
+      </c>
+      <c r="H2" s="4">
+        <f ca="1">NOW() - RAND()*70-20</f>
+        <v>41773.968260219044</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>I$1&amp;"("""&amp;A2&amp;""","""&amp;B2&amp;""","""&amp;C2&amp;""","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;", DATE(""" &amp; TEXT( G2, "yyyy-mm-dd hh:ss") &amp;""")) ; "</f>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Microsoft Xbox One","Game Console","images/Microsoft Xbox One.jpg",599,120,0, DATE("2014-06-19 21:55")) ; </v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>59</v>
@@ -551,16 +591,27 @@
       <c r="F3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="4">
+        <v>41768.059466293926</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="G3:H14" ca="1" si="0">NOW() - RAND()*70-20</f>
+        <v>41783.96568586403</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I14" si="1">I$1&amp;"("""&amp;A3&amp;""","""&amp;B3&amp;""","""&amp;C3&amp;""","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;", DATE(""" &amp; TEXT( G3, "yyyy-mm-dd hh:ss") &amp;""")) ; "</f>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Batman Arkham Knight","XBOX ONE Game","images/Batman Arkham Knight.jpg",59,30,0, DATE("2014-05-09 01:38")) ; </v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2">
         <v>59</v>
@@ -571,16 +622,27 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="4">
+        <v>41792.966339211082</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41810.308133500468</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Destiny ","XBOX ONE Game","images/Destiny - Xbox One.jpg",59,6,0, DATE("2014-06-02 23:32")) ; </v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2">
         <v>59</v>
@@ -591,16 +653,27 @@
       <c r="F5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="4">
+        <v>41756.882740894238</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41770.289315960217</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("NBA 2K14","XBOX ONE Game","images/NBA 2K14 - Xbox One.jpg",59,5,0, DATE("2014-04-27 21:09")) ; </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2">
         <v>59</v>
@@ -611,155 +684,264 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G6" s="4">
+        <v>41792.607374615509</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41771.902594479812</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Plants vs. Zombies Garden Warfare","XBOX ONE Game","images/Plants vs. Zombies Garden Warfare - Xbox One.jpg",59,4,0, DATE("2014-06-02 14:37")) ; </v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2">
+        <v>299</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>41810.50161183509</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41793.80435419672</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Sony Playstation 4","Game Console","images/Sony - Playstation 4.jpg",299,3,0, DATE("2014-06-20 12:19")) ; </v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2">
+        <v>59</v>
+      </c>
       <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>41808.6445773757</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41789.653340376855</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("The Last of Us Remastered","PlayStation 4","images/The Last of Us Remastered - PlayStation 4.jpg",59,7,0, DATE("2014-06-18 15:11")) ; </v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2">
+        <v>59</v>
+      </c>
+      <c r="E9" s="1">
         <v>20</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2">
-        <v>299</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3</v>
-      </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="4">
+        <v>41807.402587179902</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41825.319276229617</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Watch Dogs","PlayStation 4","images/Watch Dogs - PlayStation 4.jpg",59,20,0, DATE("2014-06-17 09:44")) ; </v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2">
         <v>59</v>
       </c>
       <c r="E10" s="1">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="4">
+        <v>41824.741066656497</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41761.289562778809</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Call of Duty Ghosts ","PlayStation 4","images/Call of Duty Ghosts - PlayStation 4.jpg",59,18,0, DATE("2014-07-04 17:08")) ; </v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2">
         <v>59</v>
       </c>
       <c r="E11" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="4">
+        <v>41798.225831655189</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41757.349556119385</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Infamous Second Son","PlayStation 4","images/Infamous Second Son - PlayStation 4.jpg",59,10,0, DATE("2014-06-08 05:12")) ; </v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2">
         <v>59</v>
       </c>
       <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>41802.503124383235</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41820.009655705951</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("FIFA Soccer 14","PlayStation 4","images/FIFA Soccer 14 (PS4).jpg",59,5,0, DATE("2014-06-12 12:30")) ; </v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>999.95</v>
+      </c>
+      <c r="E13" s="1">
         <v>18</v>
       </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>41763.102283467844</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41760.887901293041</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("LG - 65 inch LED - 240Hz - Smart - 3D - HDTV","Flat Screen","images/LG - 65 inch Class (64-5 a half 8inch Diag.) - LED - 4K Ultra HD TV (2160p) - 240Hz - Smart - 3D - HDTV.jpg",999.95,18,0, DATE("2014-05-04 02:17")) ; </v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2">
-        <v>59</v>
-      </c>
-      <c r="E13" s="1">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2">
-        <v>59</v>
+        <v>32</v>
+      </c>
+      <c r="D14" s="3">
+        <v>679.99</v>
       </c>
       <c r="E14" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
+      <c r="G14" s="4">
+        <v>41824.019010920259</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>41769.571744354311</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">insert into inventory(itemname ,description ,pathtoimage ,price ,numberinstock ,backordered,arrivaldate) values ("Samsung - 40 inch  LED-LCD TV - 1080p - HDTV","Flat Screen","images/Samsung - 40 inch Class (40 inch Diag.) - LED-LCD TV - 1080p - HDTV 1080p.jpg",679.99,12,0, DATE("2014-07-04 00:23")) ; </v>
       </c>
     </row>
   </sheetData>
@@ -769,24 +951,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>